<commit_message>
Updated TI parts list. READY TO ORDER
</commit_message>
<xml_diff>
--- a/MasterPartsList_Budget.xlsx
+++ b/MasterPartsList_Budget.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Senior Design\GroBot_DesignFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="24920" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="-15" yWindow="0" windowWidth="24915" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$F$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$F$15</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -88,6 +93,39 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Relay Switch</t>
+  </si>
+  <si>
+    <t>DC Power Supply</t>
+  </si>
+  <si>
+    <t>www.mouser.com</t>
+  </si>
+  <si>
+    <t>Dual 20-V N-Channel NexFet Power MOSFET</t>
+  </si>
+  <si>
+    <t>CSD85312Q3E</t>
+  </si>
+  <si>
+    <t>Dual N-Channel NexFet Power MOSFET</t>
+  </si>
+  <si>
+    <t>CSD85301Q2</t>
+  </si>
+  <si>
+    <t>Phase Dimmable PFC Flyback Controller</t>
+  </si>
+  <si>
+    <t>LM3447</t>
+  </si>
+  <si>
+    <t>Something</t>
+  </si>
+  <si>
+    <t>TI:</t>
   </si>
 </sst>
 </file>
@@ -95,8 +133,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -148,16 +186,19 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -166,6 +207,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -491,31 +540,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="48.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.875" customWidth="1"/>
+    <col min="3" max="3" width="48.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="4"/>
+    <col min="5" max="5" width="7.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -534,11 +583,11 @@
       <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -557,12 +606,12 @@
       <c r="F4">
         <v>6</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <f>E4*F4</f>
         <v>4.1399999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -581,12 +630,12 @@
       <c r="F5">
         <v>14</v>
       </c>
-      <c r="G5" s="4">
-        <f t="shared" ref="G5:G32" si="0">E5*F5</f>
+      <c r="G5" s="3">
+        <f t="shared" ref="G5:G14" si="0">E5*F5</f>
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -605,12 +654,12 @@
       <c r="F6">
         <v>4</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <f t="shared" si="0"/>
         <v>6.16</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -626,12 +675,12 @@
       <c r="F7">
         <v>2</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -647,175 +696,166 @@
       <c r="F8">
         <v>3</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="0"/>
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" ref="G10" si="1">E10*F10</f>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2.09</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" ref="G11" si="2">E11*F11</f>
+        <v>8.36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C12" t="s">
         <v>19</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D12" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E12" s="1">
         <v>17.850000000000001</v>
       </c>
-      <c r="F9">
+      <c r="F12">
         <v>8</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G12" s="3">
         <f t="shared" si="0"/>
         <v>142.80000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="G10" s="4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>9</v>
+      </c>
+      <c r="G13" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="G11" s="4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="1">
+        <v>45</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="G12" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="G13" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="G14" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="G15" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="G16" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="7:7">
-      <c r="G17" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="7:7">
-      <c r="G18" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="7:7">
-      <c r="G19" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="7:7">
-      <c r="G20" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="7:7">
-      <c r="G21" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="7:7">
-      <c r="G22" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="7:7">
-      <c r="G23" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="7:7">
-      <c r="G24" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="7:7">
-      <c r="G25" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="7:7">
-      <c r="G26" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="7:7">
-      <c r="G27" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="7:7">
-      <c r="G28" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="7:7">
-      <c r="G29" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="7:7">
-      <c r="G30" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="7:7">
-      <c r="G31" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="7:7">
-      <c r="G32" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="3">
+        <f>SUM(G4:G14)</f>
+        <v>425.46000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="3">
+        <f>SUM(G4:G11)</f>
+        <v>165.66000000000003</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:F8">
+  <autoFilter ref="A3:F15">
     <sortState ref="A4:F8">
       <sortCondition ref="E3:E8"/>
     </sortState>
@@ -829,7 +869,12 @@
     <hyperlink ref="B5" r:id="rId3"/>
     <hyperlink ref="B6" r:id="rId4"/>
     <hyperlink ref="B4" r:id="rId5"/>
-    <hyperlink ref="B9" r:id="rId6"/>
+    <hyperlink ref="B12" r:id="rId6"/>
+    <hyperlink ref="B13" r:id="rId7"/>
+    <hyperlink ref="B14" r:id="rId8"/>
+    <hyperlink ref="B9" r:id="rId9"/>
+    <hyperlink ref="B10" r:id="rId10"/>
+    <hyperlink ref="B11" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Updated budget list, not the official copy sent in
</commit_message>
<xml_diff>
--- a/MasterPartsList_Budget.xlsx
+++ b/MasterPartsList_Budget.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24500" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$F$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$G$14</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Item Name</t>
   </si>
   <si>
-    <t>Part Number</t>
-  </si>
-  <si>
     <t>Price</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Relay Switch</t>
-  </si>
-  <si>
     <t>DC Power Supply</t>
   </si>
   <si>
@@ -105,16 +99,46 @@
     <t>LM3447</t>
   </si>
   <si>
-    <t>Something</t>
-  </si>
-  <si>
-    <t>TI:</t>
-  </si>
-  <si>
     <t>SEPIC Converter (for LED)</t>
   </si>
   <si>
     <t>TPS55340</t>
+  </si>
+  <si>
+    <t>Buck DC/DC converter</t>
+  </si>
+  <si>
+    <t>Ordered</t>
+  </si>
+  <si>
+    <t>TPS54340DDAR</t>
+  </si>
+  <si>
+    <t>Cincon</t>
+  </si>
+  <si>
+    <t>418-CFM40S240</t>
+  </si>
+  <si>
+    <t>Website Part Number</t>
+  </si>
+  <si>
+    <t>Manufacturer Part #</t>
+  </si>
+  <si>
+    <t>CFM40S240</t>
+  </si>
+  <si>
+    <t>558-CX240D5</t>
+  </si>
+  <si>
+    <t>CX240D5</t>
+  </si>
+  <si>
+    <t>Solid State Relay</t>
+  </si>
+  <si>
+    <t>Crydom</t>
   </si>
 </sst>
 </file>
@@ -122,10 +146,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -144,6 +168,7 @@
       <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -153,6 +178,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF555555"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -175,18 +218,23 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -529,316 +577,359 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="48.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" style="3"/>
+    <col min="2" max="2" width="15.875" customWidth="1"/>
+    <col min="3" max="3" width="48.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.25" customWidth="1"/>
+    <col min="5" max="5" width="14.125" customWidth="1"/>
+    <col min="6" max="6" width="7.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.5">
+    <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B1" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="F1" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="1">
+        <v>4.63</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <f>F4*G4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.54</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" s="3">
+        <f t="shared" ref="H5:H14" si="0">F5*G5</f>
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1">
+        <v>17</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>30</v>
+      </c>
+      <c r="G7">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="1">
-        <v>4.63</v>
-      </c>
-      <c r="F4">
-        <v>12</v>
-      </c>
-      <c r="G4" s="3">
-        <f>E4*F4</f>
-        <v>55.56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1.54</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5" s="3">
-        <f t="shared" ref="G5:G13" si="0">E5*F5</f>
-        <v>6.16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1">
-        <v>17</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" s="3">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="1">
-        <v>30</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="I7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="1">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="1">
         <v>1.45</v>
       </c>
-      <c r="F8">
-        <v>4</v>
-      </c>
-      <c r="G8" s="3">
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8" s="3">
         <f t="shared" si="0"/>
         <v>5.8</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" ref="H9" si="1">F9*G9</f>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2.09</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" ref="H10:H11" si="2">F10*G10</f>
+        <v>8.36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="G11">
         <v>5</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="H11" s="3">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="F9">
-        <v>4</v>
-      </c>
-      <c r="G9" s="3">
-        <f t="shared" ref="G9" si="1">E9*F9</f>
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="1">
-        <v>2.09</v>
-      </c>
-      <c r="F10">
-        <v>4</v>
-      </c>
-      <c r="G10" s="3">
-        <f t="shared" ref="G10" si="2">E10*F10</f>
-        <v>8.36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
+      <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E12" t="s">
         <v>15</v>
       </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="1">
+      <c r="F12" s="1">
         <v>17.850000000000001</v>
       </c>
-      <c r="F11">
+      <c r="G12">
         <v>8</v>
       </c>
-      <c r="G11" s="3">
+      <c r="H12" s="3">
         <f t="shared" si="0"/>
         <v>142.80000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="1">
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="1">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="G13">
         <v>3</v>
       </c>
-      <c r="F12">
-        <v>9</v>
-      </c>
-      <c r="G12" s="3">
+      <c r="H13" s="3">
         <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="1">
-        <v>45</v>
-      </c>
-      <c r="F13">
+        <v>56.699999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="1">
+        <v>14.42</v>
+      </c>
+      <c r="G14">
         <v>2</v>
       </c>
-      <c r="G13" s="3">
+      <c r="H14" s="3">
         <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="G14" s="3">
-        <f>SUM(G4:G13)</f>
-        <v>445.88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="F15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="3">
-        <f>SUM(G4:G10)</f>
-        <v>186.07999999999998</v>
+        <v>28.84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G15" s="4"/>
+      <c r="H15" s="3">
+        <f>SUM(H4:H14)</f>
+        <v>362.85999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H16" s="3">
+        <f>SUM(H4:H10)</f>
+        <v>113.52</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:F14">
-    <sortState ref="A4:F8">
-      <sortCondition ref="E3:E8"/>
+  <autoFilter ref="A3:G14">
+    <sortState ref="A4:G8">
+      <sortCondition ref="F3:F8"/>
     </sortState>
   </autoFilter>
   <mergeCells count="1">
-    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B1:F1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1"/>
     <hyperlink ref="B6" r:id="rId2"/>
     <hyperlink ref="B5" r:id="rId3"/>
     <hyperlink ref="B4" r:id="rId4"/>
-    <hyperlink ref="B11" r:id="rId5"/>
-    <hyperlink ref="B12" r:id="rId6"/>
-    <hyperlink ref="B13" r:id="rId7"/>
-    <hyperlink ref="B8" r:id="rId8"/>
-    <hyperlink ref="B9" r:id="rId9"/>
-    <hyperlink ref="B10" r:id="rId10"/>
+    <hyperlink ref="B12" r:id="rId5"/>
+    <hyperlink ref="B13" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
+    <hyperlink ref="B11" r:id="rId10"/>
+    <hyperlink ref="B14" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>